<commit_message>
Enhance date utilities and loan calculations; add UTC to local date conversion and update loan function parameters for clarity
</commit_message>
<xml_diff>
--- a/test/lib_test/loan.asset_src.xlsx
+++ b/test/lib_test/loan.asset_src.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6E191C5-244E-4B71-A3B0-D43B87E8CD84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F792EFE-72BC-49EA-8BD8-DF022E6D727C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{8133C24C-105D-4170-89C8-2DFFA12ECA8A}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{8133C24C-105D-4170-89C8-2DFFA12ECA8A}"/>
   </bookViews>
   <sheets>
     <sheet name="v3" sheetId="93" r:id="rId1"/>
@@ -491,28 +491,28 @@
   <dimension ref="A1:E82"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="13" style="1" customWidth="1"/>
-    <col min="2" max="2" width="12.734375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="13.15625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="16.734375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="16.5234375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="12.7265625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="13.1796875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="16.7265625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="16.54296875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>9</v>
       </c>
       <c r="B1" s="10">
-        <f>B10</f>
-        <v>44661</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+        <f>B11</f>
+        <v>44691</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
         <v>2</v>
       </c>
@@ -527,7 +527,7 @@
         <v>1810.2316000000001</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
         <v>5</v>
       </c>
@@ -535,7 +535,7 @@
         <v>3.3000000000000002E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
         <v>6</v>
       </c>
@@ -543,7 +543,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
         <v>7</v>
       </c>
@@ -552,7 +552,7 @@
       </c>
       <c r="E5" s="6"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
         <v>10</v>
       </c>
@@ -562,7 +562,7 @@
       </c>
       <c r="E6" s="6"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
         <v>11</v>
       </c>
@@ -572,7 +572,7 @@
       </c>
       <c r="E7" s="6"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -589,7 +589,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>0</v>
       </c>
@@ -607,12 +607,12 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>0</v>
       </c>
       <c r="B11" s="2">
-        <v>44661</v>
+        <v>44691</v>
       </c>
       <c r="C11" s="7">
         <v>0</v>
@@ -626,12 +626,12 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>0</v>
       </c>
       <c r="B12" s="2">
-        <v>44691</v>
+        <v>44722</v>
       </c>
       <c r="C12" s="7">
         <v>0</v>
@@ -645,12 +645,12 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>0</v>
       </c>
       <c r="B13" s="2">
-        <v>44722</v>
+        <v>44752</v>
       </c>
       <c r="C13" s="7">
         <v>0</v>
@@ -664,12 +664,12 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>0</v>
       </c>
       <c r="B14" s="2">
-        <v>44752</v>
+        <v>44783</v>
       </c>
       <c r="C14" s="7">
         <v>0</v>
@@ -683,12 +683,12 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>0</v>
       </c>
       <c r="B15" s="2">
-        <v>44783</v>
+        <v>44814</v>
       </c>
       <c r="C15" s="7">
         <v>0</v>
@@ -702,12 +702,12 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <v>0</v>
       </c>
       <c r="B16" s="2">
-        <v>44814</v>
+        <v>44844</v>
       </c>
       <c r="C16" s="7">
         <v>0</v>
@@ -721,12 +721,12 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
         <v>0</v>
       </c>
       <c r="B17" s="2">
-        <v>44844</v>
+        <v>44875</v>
       </c>
       <c r="C17" s="7">
         <v>0</v>
@@ -740,12 +740,12 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
         <v>0</v>
       </c>
       <c r="B18" s="2">
-        <v>44875</v>
+        <v>44905</v>
       </c>
       <c r="C18" s="7">
         <v>0</v>
@@ -759,12 +759,12 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
         <v>0</v>
       </c>
       <c r="B19" s="2">
-        <v>44905</v>
+        <v>44936</v>
       </c>
       <c r="C19" s="7">
         <v>0</v>
@@ -778,12 +778,12 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
         <v>0</v>
       </c>
       <c r="B20" s="2">
-        <v>44936</v>
+        <v>44967</v>
       </c>
       <c r="C20" s="7">
         <v>0</v>
@@ -797,12 +797,12 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="1">
         <v>0</v>
       </c>
       <c r="B21" s="2">
-        <v>44967</v>
+        <v>44995</v>
       </c>
       <c r="C21" s="7">
         <v>0</v>
@@ -816,12 +816,12 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="1">
         <v>0</v>
       </c>
       <c r="B22" s="2">
-        <v>44995</v>
+        <v>45026</v>
       </c>
       <c r="C22" s="7">
         <v>0</v>
@@ -835,12 +835,12 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" s="1">
         <v>0</v>
       </c>
       <c r="B23" s="2">
-        <v>45026</v>
+        <v>45056</v>
       </c>
       <c r="C23" s="7">
         <f>ROUND($D$2-D23,4)</f>
@@ -855,12 +855,12 @@
         <v>98464.768400000001</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" s="1">
         <v>1</v>
       </c>
       <c r="B24" s="2">
-        <v>45056</v>
+        <v>45087</v>
       </c>
       <c r="C24" s="7">
         <f t="shared" ref="C24:C82" si="2">ROUND($D$2-D24,4)</f>
@@ -875,12 +875,12 @@
         <v>96925.314899999998</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" s="1">
         <v>2</v>
       </c>
       <c r="B25" s="2">
-        <v>45087</v>
+        <v>45117</v>
       </c>
       <c r="C25" s="7">
         <f t="shared" si="2"/>
@@ -895,12 +895,12 @@
         <v>95381.627899999992</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" s="1">
         <v>3</v>
       </c>
       <c r="B26" s="2">
-        <v>45117</v>
+        <v>45148</v>
       </c>
       <c r="C26" s="7">
         <f t="shared" si="2"/>
@@ -915,12 +915,12 @@
         <v>93833.695799999987</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" s="1">
         <v>4</v>
       </c>
       <c r="B27" s="2">
-        <v>45148</v>
+        <v>45179</v>
       </c>
       <c r="C27" s="7">
         <f t="shared" si="2"/>
@@ -935,12 +935,12 @@
         <v>92281.506899999993</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" s="1">
         <v>5</v>
       </c>
       <c r="B28" s="2">
-        <v>45179</v>
+        <v>45209</v>
       </c>
       <c r="C28" s="7">
         <f t="shared" si="2"/>
@@ -955,12 +955,12 @@
         <v>90725.049399999989</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" s="1">
         <v>6</v>
       </c>
       <c r="B29" s="2">
-        <v>45209</v>
+        <v>45240</v>
       </c>
       <c r="C29" s="7">
         <f t="shared" si="2"/>
@@ -975,12 +975,12 @@
         <v>89164.311699999991</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" s="1">
         <v>7</v>
       </c>
       <c r="B30" s="2">
-        <v>45240</v>
+        <v>45270</v>
       </c>
       <c r="C30" s="7">
         <f t="shared" si="2"/>
@@ -995,12 +995,12 @@
         <v>87599.281999999992</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" s="1">
         <v>8</v>
       </c>
       <c r="B31" s="2">
-        <v>45270</v>
+        <v>45301</v>
       </c>
       <c r="C31" s="7">
         <f t="shared" si="2"/>
@@ -1015,12 +1015,12 @@
         <v>86029.948399999994</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" s="1">
         <v>9</v>
       </c>
       <c r="B32" s="2">
-        <v>45301</v>
+        <v>45332</v>
       </c>
       <c r="C32" s="7">
         <f t="shared" si="2"/>
@@ -1035,12 +1035,12 @@
         <v>84456.299199999994</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" s="1">
         <v>10</v>
       </c>
       <c r="B33" s="2">
-        <v>45332</v>
+        <v>45361</v>
       </c>
       <c r="C33" s="7">
         <f t="shared" si="2"/>
@@ -1055,12 +1055,12 @@
         <v>82878.32239999999</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" s="1">
         <v>11</v>
       </c>
       <c r="B34" s="2">
-        <v>45361</v>
+        <v>45392</v>
       </c>
       <c r="C34" s="7">
         <f t="shared" si="2"/>
@@ -1075,12 +1075,12 @@
         <v>81296.006199999989</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" s="1">
         <v>12</v>
       </c>
       <c r="B35" s="2">
-        <v>45392</v>
+        <v>45422</v>
       </c>
       <c r="C35" s="7">
         <f t="shared" si="2"/>
@@ -1095,12 +1095,12 @@
         <v>79709.338599999988</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" s="1">
         <v>13</v>
       </c>
       <c r="B36" s="2">
-        <v>45422</v>
+        <v>45453</v>
       </c>
       <c r="C36" s="7">
         <f t="shared" si="2"/>
@@ -1115,12 +1115,12 @@
         <v>78118.30769999999</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37" s="1">
         <v>14</v>
       </c>
       <c r="B37" s="2">
-        <v>45453</v>
+        <v>45483</v>
       </c>
       <c r="C37" s="7">
         <f t="shared" si="2"/>
@@ -1135,12 +1135,12 @@
         <v>76522.901399999988</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38" s="1">
         <v>15</v>
       </c>
       <c r="B38" s="2">
-        <v>45483</v>
+        <v>45514</v>
       </c>
       <c r="C38" s="7">
         <f t="shared" si="2"/>
@@ -1155,12 +1155,12 @@
         <v>74923.107799999983</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39" s="1">
         <v>16</v>
       </c>
       <c r="B39" s="2">
-        <v>45514</v>
+        <v>45545</v>
       </c>
       <c r="C39" s="7">
         <f t="shared" si="2"/>
@@ -1175,12 +1175,12 @@
         <v>73318.914699999979</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A40" s="1">
         <v>17</v>
       </c>
       <c r="B40" s="2">
-        <v>45545</v>
+        <v>45575</v>
       </c>
       <c r="C40" s="7">
         <f t="shared" si="2"/>
@@ -1195,12 +1195,12 @@
         <v>71710.310099999973</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A41" s="1">
         <v>18</v>
       </c>
       <c r="B41" s="2">
-        <v>45575</v>
+        <v>45606</v>
       </c>
       <c r="C41" s="7">
         <f t="shared" si="2"/>
@@ -1215,12 +1215,12 @@
         <v>70097.281899999973</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A42" s="1">
         <v>19</v>
       </c>
       <c r="B42" s="2">
-        <v>45606</v>
+        <v>45636</v>
       </c>
       <c r="C42" s="7">
         <f t="shared" si="2"/>
@@ -1235,12 +1235,12 @@
         <v>68479.817799999975</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A43" s="1">
         <v>20</v>
       </c>
       <c r="B43" s="2">
-        <v>45636</v>
+        <v>45667</v>
       </c>
       <c r="C43" s="7">
         <f t="shared" si="2"/>
@@ -1255,12 +1255,12 @@
         <v>66857.905699999974</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A44" s="1">
         <v>21</v>
       </c>
       <c r="B44" s="2">
-        <v>45667</v>
+        <v>45698</v>
       </c>
       <c r="C44" s="7">
         <f t="shared" si="2"/>
@@ -1275,12 +1275,12 @@
         <v>65231.533299999974</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A45" s="1">
         <v>22</v>
       </c>
       <c r="B45" s="2">
-        <v>45698</v>
+        <v>45726</v>
       </c>
       <c r="C45" s="7">
         <f t="shared" si="2"/>
@@ -1295,12 +1295,12 @@
         <v>63600.68839999997</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A46" s="1">
         <v>23</v>
       </c>
       <c r="B46" s="2">
-        <v>45726</v>
+        <v>45757</v>
       </c>
       <c r="C46" s="7">
         <f t="shared" si="2"/>
@@ -1315,12 +1315,12 @@
         <v>61965.358699999968</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A47" s="1">
         <v>24</v>
       </c>
       <c r="B47" s="2">
-        <v>45757</v>
+        <v>45787</v>
       </c>
       <c r="C47" s="7">
         <f t="shared" si="2"/>
@@ -1335,12 +1335,12 @@
         <v>60325.531799999968</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A48" s="1">
         <v>25</v>
       </c>
       <c r="B48" s="2">
-        <v>45787</v>
+        <v>45818</v>
       </c>
       <c r="C48" s="7">
         <f t="shared" si="2"/>
@@ -1355,12 +1355,12 @@
         <v>58681.195399999968</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A49" s="1">
         <v>26</v>
       </c>
       <c r="B49" s="2">
-        <v>45818</v>
+        <v>45848</v>
       </c>
       <c r="C49" s="7">
         <f t="shared" si="2"/>
@@ -1375,12 +1375,12 @@
         <v>57032.337099999968</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A50" s="1">
         <v>27</v>
       </c>
       <c r="B50" s="2">
-        <v>45848</v>
+        <v>45879</v>
       </c>
       <c r="C50" s="7">
         <f t="shared" si="2"/>
@@ -1395,12 +1395,12 @@
         <v>55378.944399999971</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A51" s="1">
         <v>28</v>
       </c>
       <c r="B51" s="2">
-        <v>45879</v>
+        <v>45910</v>
       </c>
       <c r="C51" s="7">
         <f t="shared" si="2"/>
@@ -1415,12 +1415,12 @@
         <v>53721.004899999971</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A52" s="1">
         <v>29</v>
       </c>
       <c r="B52" s="2">
-        <v>45910</v>
+        <v>45940</v>
       </c>
       <c r="C52" s="7">
         <f t="shared" si="2"/>
@@ -1435,12 +1435,12 @@
         <v>52058.50609999997</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A53" s="1">
         <v>30</v>
       </c>
       <c r="B53" s="2">
-        <v>45940</v>
+        <v>45971</v>
       </c>
       <c r="C53" s="7">
         <f t="shared" si="2"/>
@@ -1455,12 +1455,12 @@
         <v>50391.435399999973</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A54" s="1">
         <v>31</v>
       </c>
       <c r="B54" s="2">
-        <v>45971</v>
+        <v>46001</v>
       </c>
       <c r="C54" s="7">
         <f t="shared" si="2"/>
@@ -1475,12 +1475,12 @@
         <v>48719.780199999972</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A55" s="1">
         <v>32</v>
       </c>
       <c r="B55" s="2">
-        <v>46001</v>
+        <v>46032</v>
       </c>
       <c r="C55" s="7">
         <f t="shared" si="2"/>
@@ -1495,12 +1495,12 @@
         <v>47043.527999999969</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A56" s="1">
         <v>33</v>
       </c>
       <c r="B56" s="2">
-        <v>46032</v>
+        <v>46063</v>
       </c>
       <c r="C56" s="7">
         <f t="shared" si="2"/>
@@ -1515,12 +1515,12 @@
         <v>45362.666099999966</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A57" s="1">
         <v>34</v>
       </c>
       <c r="B57" s="2">
-        <v>46063</v>
+        <v>46091</v>
       </c>
       <c r="C57" s="7">
         <f t="shared" si="2"/>
@@ -1535,12 +1535,12 @@
         <v>43677.181799999962</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A58" s="1">
         <v>35</v>
       </c>
       <c r="B58" s="2">
-        <v>46091</v>
+        <v>46122</v>
       </c>
       <c r="C58" s="7">
         <f t="shared" si="2"/>
@@ -1555,12 +1555,12 @@
         <v>41987.062399999959</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A59" s="1">
         <v>36</v>
       </c>
       <c r="B59" s="2">
-        <v>46122</v>
+        <v>46152</v>
       </c>
       <c r="C59" s="7">
         <f t="shared" si="2"/>
@@ -1575,12 +1575,12 @@
         <v>40292.295199999957</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A60" s="1">
         <v>37</v>
       </c>
       <c r="B60" s="2">
-        <v>46152</v>
+        <v>46183</v>
       </c>
       <c r="C60" s="7">
         <f t="shared" si="2"/>
@@ -1595,12 +1595,12 @@
         <v>38592.867399999959</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A61" s="1">
         <v>38</v>
       </c>
       <c r="B61" s="2">
-        <v>46183</v>
+        <v>46213</v>
       </c>
       <c r="C61" s="7">
         <f t="shared" si="2"/>
@@ -1615,12 +1615,12 @@
         <v>36888.766199999962</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A62" s="1">
         <v>39</v>
       </c>
       <c r="B62" s="2">
-        <v>46213</v>
+        <v>46244</v>
       </c>
       <c r="C62" s="7">
         <f t="shared" si="2"/>
@@ -1635,12 +1635,12 @@
         <v>35179.978699999963</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A63" s="1">
         <v>40</v>
       </c>
       <c r="B63" s="2">
-        <v>46244</v>
+        <v>46275</v>
       </c>
       <c r="C63" s="7">
         <f t="shared" si="2"/>
@@ -1655,12 +1655,12 @@
         <v>33466.491999999962</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A64" s="1">
         <v>41</v>
       </c>
       <c r="B64" s="2">
-        <v>46275</v>
+        <v>46305</v>
       </c>
       <c r="C64" s="7">
         <f t="shared" si="2"/>
@@ -1675,12 +1675,12 @@
         <v>31748.293299999961</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A65" s="1">
         <v>42</v>
       </c>
       <c r="B65" s="2">
-        <v>46305</v>
+        <v>46336</v>
       </c>
       <c r="C65" s="7">
         <f t="shared" si="2"/>
@@ -1695,12 +1695,12 @@
         <v>30025.369499999961</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A66" s="1">
         <v>43</v>
       </c>
       <c r="B66" s="2">
-        <v>46336</v>
+        <v>46366</v>
       </c>
       <c r="C66" s="7">
         <f t="shared" si="2"/>
@@ -1715,12 +1715,12 @@
         <v>28297.707699999959</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A67" s="1">
         <v>44</v>
       </c>
       <c r="B67" s="2">
-        <v>46366</v>
+        <v>46397</v>
       </c>
       <c r="C67" s="7">
         <f t="shared" si="2"/>
@@ -1735,12 +1735,12 @@
         <v>26565.29479999996</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A68" s="1">
         <v>45</v>
       </c>
       <c r="B68" s="2">
-        <v>46397</v>
+        <v>46428</v>
       </c>
       <c r="C68" s="7">
         <f t="shared" si="2"/>
@@ -1755,12 +1755,12 @@
         <v>24828.11779999996</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A69" s="1">
         <v>46</v>
       </c>
       <c r="B69" s="2">
-        <v>46428</v>
+        <v>46456</v>
       </c>
       <c r="C69" s="7">
         <f t="shared" si="2"/>
@@ -1775,12 +1775,12 @@
         <v>23086.163499999959</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A70" s="1">
         <v>47</v>
       </c>
       <c r="B70" s="2">
-        <v>46456</v>
+        <v>46487</v>
       </c>
       <c r="C70" s="7">
         <f t="shared" si="2"/>
@@ -1795,12 +1795,12 @@
         <v>21339.418799999959</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A71" s="1">
         <v>48</v>
       </c>
       <c r="B71" s="2">
-        <v>46487</v>
+        <v>46517</v>
       </c>
       <c r="C71" s="7">
         <f t="shared" si="2"/>
@@ -1815,12 +1815,12 @@
         <v>19587.870599999958</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A72" s="1">
         <v>49</v>
       </c>
       <c r="B72" s="2">
-        <v>46517</v>
+        <v>46548</v>
       </c>
       <c r="C72" s="7">
         <f t="shared" si="2"/>
@@ -1835,12 +1835,12 @@
         <v>17831.505599999957</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A73" s="1">
         <v>50</v>
       </c>
       <c r="B73" s="2">
-        <v>46548</v>
+        <v>46578</v>
       </c>
       <c r="C73" s="7">
         <f t="shared" si="2"/>
@@ -1855,12 +1855,12 @@
         <v>16070.310599999957</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A74" s="1">
         <v>51</v>
       </c>
       <c r="B74" s="2">
-        <v>46578</v>
+        <v>46609</v>
       </c>
       <c r="C74" s="7">
         <f t="shared" si="2"/>
@@ -1875,12 +1875,12 @@
         <v>14304.272399999958</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A75" s="1">
         <v>52</v>
       </c>
       <c r="B75" s="2">
-        <v>46609</v>
+        <v>46640</v>
       </c>
       <c r="C75" s="7">
         <f t="shared" si="2"/>
@@ -1895,12 +1895,12 @@
         <v>12533.377499999959</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A76" s="1">
         <v>53</v>
       </c>
       <c r="B76" s="2">
-        <v>46640</v>
+        <v>46670</v>
       </c>
       <c r="C76" s="7">
         <f t="shared" si="2"/>
@@ -1915,12 +1915,12 @@
         <v>10757.612699999958</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A77" s="1">
         <v>54</v>
       </c>
       <c r="B77" s="2">
-        <v>46670</v>
+        <v>46701</v>
       </c>
       <c r="C77" s="7">
         <f t="shared" si="2"/>
@@ -1935,12 +1935,12 @@
         <v>8976.9644999999582</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A78" s="1">
         <v>55</v>
       </c>
       <c r="B78" s="2">
-        <v>46701</v>
+        <v>46731</v>
       </c>
       <c r="C78" s="7">
         <f t="shared" si="2"/>
@@ -1955,12 +1955,12 @@
         <v>7191.4195999999583</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A79" s="1">
         <v>56</v>
       </c>
       <c r="B79" s="2">
-        <v>46731</v>
+        <v>46762</v>
       </c>
       <c r="C79" s="7">
         <f t="shared" si="2"/>
@@ -1975,12 +1975,12 @@
         <v>5400.964399999958</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A80" s="1">
         <v>57</v>
       </c>
       <c r="B80" s="2">
-        <v>46762</v>
+        <v>46793</v>
       </c>
       <c r="C80" s="7">
         <f t="shared" si="2"/>
@@ -1995,12 +1995,12 @@
         <v>3605.5854999999583</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A81" s="1">
         <v>58</v>
       </c>
       <c r="B81" s="2">
-        <v>46793</v>
+        <v>46822</v>
       </c>
       <c r="C81" s="7">
         <f t="shared" si="2"/>
@@ -2015,12 +2015,12 @@
         <v>1805.2692999999583</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A82" s="1">
         <v>59</v>
       </c>
       <c r="B82" s="2">
-        <v>46822</v>
+        <v>46853</v>
       </c>
       <c r="C82" s="7">
         <f t="shared" si="2"/>

</xml_diff>